<commit_message>
Rastertunnelmikroskop aufgabe c und d
</commit_message>
<xml_diff>
--- a/Vincent/Rastertunnelmikroskopie/Abstand_atome.xlsx
+++ b/Vincent/Rastertunnelmikroskopie/Abstand_atome.xlsx
@@ -377,7 +377,7 @@
   <dimension ref="C4:N24"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J28" sqref="J28"/>
+      <selection activeCell="N7" sqref="N7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -447,8 +447,8 @@
         <v>8.8214736842105257</v>
       </c>
       <c r="N6">
-        <f>1/18*SQRT(SUM(K6:K14))</f>
-        <v>0.30241977261872888</v>
+        <f>1/18*SQRT(SUM(K6:K24))</f>
+        <v>0.37326229787502613</v>
       </c>
     </row>
     <row r="7" spans="3:14" x14ac:dyDescent="0.25">
@@ -456,14 +456,14 @@
         <v>0.27</v>
       </c>
       <c r="D7">
-        <f t="shared" ref="D7:D19" si="0">(C7-$F$6)^2</f>
+        <f>(C7-$F$6)^2</f>
         <v>1.9612244897958867E-5</v>
       </c>
       <c r="J7">
         <v>10.901</v>
       </c>
       <c r="K7">
-        <f t="shared" ref="K7:K24" si="1">(J7-$M$6)^2</f>
+        <f t="shared" ref="K7:K24" si="0">(J7-$M$6)^2</f>
         <v>4.3244296980609436</v>
       </c>
     </row>
@@ -472,14 +472,14 @@
         <v>0.26400000000000001</v>
       </c>
       <c r="D8">
-        <f t="shared" si="0"/>
+        <f t="shared" ref="D7:D19" si="1">(C8-$F$6)^2</f>
         <v>2.4693877551021697E-6</v>
       </c>
       <c r="J8">
         <v>10.967000000000001</v>
       </c>
       <c r="K8">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4.603283171745157</v>
       </c>
     </row>
@@ -488,14 +488,14 @@
         <v>0.25900000000000001</v>
       </c>
       <c r="D9">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.3183673469388353E-5</v>
       </c>
       <c r="J9">
         <v>6.444</v>
       </c>
       <c r="K9">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5.6523811191135707</v>
       </c>
     </row>
@@ -504,14 +504,14 @@
         <v>0.25900000000000001</v>
       </c>
       <c r="D10">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>4.3183673469388353E-5</v>
       </c>
       <c r="J10">
         <v>8.4359999999999999</v>
       </c>
       <c r="K10">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.14858996121883614</v>
       </c>
     </row>
@@ -520,7 +520,7 @@
         <v>0.26700000000000002</v>
       </c>
       <c r="D11">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.0408163265305024E-6</v>
       </c>
       <c r="G11" t="s">
@@ -530,7 +530,7 @@
         <v>9.6750000000000007</v>
       </c>
       <c r="K11">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.72850717174515467</v>
       </c>
     </row>
@@ -539,14 +539,14 @@
         <v>0.26400000000000001</v>
       </c>
       <c r="D12">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>2.4693877551021697E-6</v>
       </c>
       <c r="J12">
         <v>11.881</v>
       </c>
       <c r="K12">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9.3607012770083156</v>
       </c>
       <c r="M12" t="s">
@@ -558,7 +558,7 @@
         <v>0.27</v>
       </c>
       <c r="D13">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.9612244897958867E-5</v>
       </c>
       <c r="G13" t="s">
@@ -568,7 +568,7 @@
         <v>6.7050000000000001</v>
       </c>
       <c r="K13">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4.4794608559556757</v>
       </c>
     </row>
@@ -577,14 +577,14 @@
         <v>0.26200000000000001</v>
       </c>
       <c r="D14">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.2755102040816632E-5</v>
       </c>
       <c r="J14">
         <v>9.0229999999999997</v>
       </c>
       <c r="K14">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>4.0612855955678796E-2</v>
       </c>
       <c r="M14" t="s">
@@ -596,14 +596,14 @@
         <v>0.27</v>
       </c>
       <c r="D15">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.9612244897958867E-5</v>
       </c>
       <c r="J15">
         <v>5.6870000000000003</v>
       </c>
       <c r="K15">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9.8249252770083046</v>
       </c>
     </row>
@@ -612,14 +612,14 @@
         <v>0.26200000000000001</v>
       </c>
       <c r="D16">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.2755102040816632E-5</v>
       </c>
       <c r="J16">
         <v>8.74</v>
       </c>
       <c r="K16">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>6.6379612188364285E-3</v>
       </c>
     </row>
@@ -628,14 +628,14 @@
         <v>0.27700000000000002</v>
       </c>
       <c r="D17">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.3061224489795852E-4</v>
       </c>
       <c r="J17">
         <v>8.5129999999999999</v>
       </c>
       <c r="K17">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>9.5156013850415194E-2</v>
       </c>
     </row>
@@ -644,14 +644,14 @@
         <v>0.26200000000000001</v>
       </c>
       <c r="D18">
-        <f t="shared" si="0"/>
+        <f t="shared" si="1"/>
         <v>1.2755102040816632E-5</v>
       </c>
       <c r="J18">
         <v>8.8290000000000006</v>
       </c>
       <c r="K18">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>5.6645429362899724E-5</v>
       </c>
     </row>
@@ -660,14 +660,14 @@
         <v>0.27</v>
       </c>
       <c r="D19">
-        <f t="shared" si="0"/>
+        <f>(C19-$F$6)^2</f>
         <v>1.9612244897958867E-5</v>
       </c>
       <c r="J19">
         <v>9.6059999999999999</v>
       </c>
       <c r="K19">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.61548154016620582</v>
       </c>
     </row>
@@ -676,7 +676,7 @@
         <v>8.7729999999999997</v>
       </c>
       <c r="K20">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2.3496980609417979E-3</v>
       </c>
     </row>
@@ -685,7 +685,7 @@
         <v>7.3710000000000004</v>
       </c>
       <c r="K21">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2.1038739085872544</v>
       </c>
     </row>
@@ -694,7 +694,7 @@
         <v>8.6709999999999994</v>
       </c>
       <c r="K22">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>2.2642329639889196E-2</v>
       </c>
     </row>
@@ -703,7 +703,7 @@
         <v>10.186999999999999</v>
       </c>
       <c r="K23">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>1.8646621191135735</v>
       </c>
     </row>
@@ -712,7 +712,7 @@
         <v>7.835</v>
       </c>
       <c r="K24">
-        <f t="shared" si="1"/>
+        <f t="shared" si="0"/>
         <v>0.97313032963988799</v>
       </c>
     </row>

</xml_diff>